<commit_message>
changes to intramural 22-23
</commit_message>
<xml_diff>
--- a/_tab_mariel_results.xlsx
+++ b/_tab_mariel_results.xlsx
@@ -38,28 +38,28 @@
     <t xml:space="preserve">Probs.</t>
   </si>
   <si>
-    <t xml:space="preserve">1_yr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98.4 (98.3,98.6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97.2 (97.1,97.4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96.6 (96.3,96.8)</t>
+    <t xml:space="preserve">1 yr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98.5 (98.3,98.6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97.3 (97.1,97.4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96.6 (96.4,96.9)</t>
   </si>
   <si>
     <t xml:space="preserve">-1.2 (-1.4,-1.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">-1.9 (-2.2,-1.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.6 (0.4,0.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3_yrs</t>
+    <t xml:space="preserve">-1.8 (-2.1,-1.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.6 (0.3,0.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 yrs</t>
   </si>
   <si>
     <t xml:space="preserve">96.4 (96.1,96.7)</t>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">94.3 (94.0,94.5)</t>
   </si>
   <si>
-    <t xml:space="preserve">93.2 (92.8,93.6)</t>
+    <t xml:space="preserve">93.2 (92.8,93.5)</t>
   </si>
   <si>
     <t xml:space="preserve">-2.2 (-2.5,-1.8)</t>
@@ -80,10 +80,10 @@
     <t xml:space="preserve">1.1 (0.6,1.5)</t>
   </si>
   <si>
-    <t xml:space="preserve">5_yrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94.9 (94.5,95.3)</t>
+    <t xml:space="preserve">5 yrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94.9 (94.6,95.3)</t>
   </si>
   <si>
     <t xml:space="preserve">92.3 (92.0,92.6)</t>
@@ -104,13 +104,13 @@
     <t xml:space="preserve">RMST</t>
   </si>
   <si>
-    <t xml:space="preserve">1.010 (1.008,1.011)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.002 (1.001,1.003)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.998 (0.997,1.000)</t>
+    <t xml:space="preserve">0.992 (0.991,0.993)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.985 (0.984,0.986)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.981 (0.979,0.982)</t>
   </si>
   <si>
     <t xml:space="preserve">-0.007 (-0.009,-0.006)</t>
@@ -122,37 +122,37 @@
     <t xml:space="preserve">0.004 (0.002,0.006)</t>
   </si>
   <si>
-    <t xml:space="preserve">2.931 (2.925,2.936)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.889 (2.884,2.893)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.867 (2.860,2.875)</t>
+    <t xml:space="preserve">2.939 (2.933,2.945)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.897 (2.893,2.902)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.876 (2.868,2.883)</t>
   </si>
   <si>
     <t xml:space="preserve">-0.042 (-0.049,-0.035)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.063 (-0.073,-0.054)</t>
+    <t xml:space="preserve">-0.064 (-0.074,-0.054)</t>
   </si>
   <si>
     <t xml:space="preserve">0.022 (0.013,0.031)</t>
   </si>
   <si>
-    <t xml:space="preserve">4.878 (4.865,4.890)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.786 (4.777,4.796)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.740 (4.724,4.755)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.091 (-0.107,-0.076)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.138 (-0.158,-0.117)</t>
+    <t xml:space="preserve">4.852 (4.840,4.864)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.761 (4.751,4.770)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.715 (4.700,4.730)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.091 (-0.106,-0.076)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.137 (-0.157,-0.116)</t>
   </si>
   <si>
     <t xml:space="preserve">0.046 (0.027,0.065)</t>

</xml_diff>